<commit_message>
split tables; redefined MFN
</commit_message>
<xml_diff>
--- a/data/ppp_2020_2023.xlsx
+++ b/data/ppp_2020_2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\price_prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\price_prediction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC735408-0B84-4776-9DDA-CDB10535062E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00DE078-75D0-4E33-B805-E7946F9F6F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Euro area (20 countries)</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   <si>
     <t>country</t>
   </si>
+  <si>
+    <t>United States of America</t>
+  </si>
 </sst>
 </file>
 
@@ -209,7 +209,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="268" x14ac:knownFonts="1">
+  <fonts count="267" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,11 +1018,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -7471,236 +7466,236 @@
     <xf numFmtId="165" fontId="190" fillId="191" borderId="190" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="191" fillId="192" borderId="191" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="191" fillId="193" borderId="192" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="192" fillId="194" borderId="193" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="193" fillId="195" borderId="194" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="194" fillId="196" borderId="195" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="195" fillId="197" borderId="196" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="4" fontId="192" fillId="193" borderId="192" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="193" fillId="194" borderId="193" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="194" fillId="195" borderId="194" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="195" fillId="196" borderId="195" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="196" fillId="197" borderId="196" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="196" fillId="198" borderId="197" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="197" fillId="199" borderId="198" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="198" fillId="200" borderId="199" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="199" fillId="201" borderId="200" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="200" fillId="202" borderId="201" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="197" fillId="198" borderId="197" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="198" fillId="199" borderId="198" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="199" fillId="200" borderId="199" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="200" fillId="201" borderId="200" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="201" fillId="202" borderId="201" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="201" fillId="203" borderId="202" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="202" fillId="204" borderId="203" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="203" fillId="205" borderId="204" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="204" fillId="206" borderId="205" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="205" fillId="207" borderId="206" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="202" fillId="203" borderId="202" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="203" fillId="204" borderId="203" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="204" fillId="205" borderId="204" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="205" fillId="206" borderId="205" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="206" fillId="207" borderId="206" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="206" fillId="208" borderId="207" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="207" fillId="209" borderId="208" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="208" fillId="210" borderId="209" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="209" fillId="211" borderId="210" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="210" fillId="212" borderId="211" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="3" fontId="207" fillId="208" borderId="207" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="208" fillId="209" borderId="208" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="209" fillId="210" borderId="209" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="210" fillId="211" borderId="210" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="211" fillId="212" borderId="211" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="211" fillId="213" borderId="212" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="212" fillId="214" borderId="213" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="213" fillId="215" borderId="214" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="214" fillId="216" borderId="215" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="215" fillId="217" borderId="216" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="212" fillId="213" borderId="212" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="213" fillId="214" borderId="213" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="214" fillId="215" borderId="214" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="215" fillId="216" borderId="215" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="216" fillId="217" borderId="216" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="216" fillId="218" borderId="217" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="217" fillId="219" borderId="218" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="218" fillId="220" borderId="219" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="219" fillId="221" borderId="220" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="220" fillId="222" borderId="221" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="217" fillId="218" borderId="217" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="218" fillId="219" borderId="218" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="219" fillId="220" borderId="219" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="220" fillId="221" borderId="220" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="221" fillId="222" borderId="221" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="221" fillId="223" borderId="222" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="222" fillId="224" borderId="223" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="223" fillId="225" borderId="224" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="224" fillId="226" borderId="225" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="225" fillId="227" borderId="226" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="222" fillId="223" borderId="222" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="223" fillId="224" borderId="223" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="224" fillId="225" borderId="224" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="225" fillId="226" borderId="225" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="226" fillId="227" borderId="226" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="226" fillId="228" borderId="227" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="227" fillId="229" borderId="228" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="228" fillId="230" borderId="229" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="229" fillId="231" borderId="230" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="230" fillId="232" borderId="231" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="227" fillId="228" borderId="227" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="228" fillId="229" borderId="228" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="229" fillId="230" borderId="229" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="230" fillId="231" borderId="230" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="231" fillId="232" borderId="231" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="231" fillId="233" borderId="232" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="232" fillId="234" borderId="233" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="233" fillId="235" borderId="234" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="234" fillId="236" borderId="235" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="235" fillId="237" borderId="236" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="4" fontId="232" fillId="233" borderId="232" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="233" fillId="234" borderId="233" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="234" fillId="235" borderId="234" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="235" fillId="236" borderId="235" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="236" fillId="237" borderId="236" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="236" fillId="238" borderId="237" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="237" fillId="239" borderId="238" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="238" fillId="240" borderId="239" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="239" fillId="241" borderId="240" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="240" fillId="242" borderId="241" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="237" fillId="238" borderId="237" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="238" fillId="239" borderId="238" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="239" fillId="240" borderId="239" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="240" fillId="241" borderId="240" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="241" fillId="242" borderId="241" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="241" fillId="243" borderId="242" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="242" fillId="244" borderId="243" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="243" fillId="245" borderId="244" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="244" fillId="246" borderId="245" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="245" fillId="247" borderId="246" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="242" fillId="243" borderId="242" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="243" fillId="244" borderId="243" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="244" fillId="245" borderId="244" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="245" fillId="246" borderId="245" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="246" fillId="247" borderId="246" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="246" fillId="248" borderId="247" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="247" fillId="249" borderId="248" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="248" fillId="250" borderId="249" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="249" fillId="251" borderId="250" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="250" fillId="252" borderId="251" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="247" fillId="248" borderId="247" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="248" fillId="249" borderId="248" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="249" fillId="250" borderId="249" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="250" fillId="251" borderId="250" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="251" fillId="252" borderId="251" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="251" fillId="253" borderId="252" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="252" fillId="254" borderId="253" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="253" fillId="255" borderId="254" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="254" fillId="256" borderId="255" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="255" fillId="257" borderId="256" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="252" fillId="253" borderId="252" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="253" fillId="254" borderId="253" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="254" fillId="255" borderId="254" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="255" fillId="256" borderId="255" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="256" fillId="257" borderId="256" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="256" fillId="258" borderId="257" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="257" fillId="259" borderId="258" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="258" fillId="260" borderId="259" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="259" fillId="261" borderId="260" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="260" fillId="262" borderId="261" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="257" fillId="258" borderId="257" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="258" fillId="259" borderId="258" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="259" fillId="260" borderId="259" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="260" fillId="261" borderId="260" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="261" fillId="262" borderId="261" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="261" fillId="263" borderId="262" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="262" fillId="264" borderId="263" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="263" fillId="265" borderId="264" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="264" fillId="266" borderId="265" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="265" fillId="267" borderId="266" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="266" fillId="268" borderId="267" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="262" fillId="263" borderId="262" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="263" fillId="264" borderId="263" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="264" fillId="265" borderId="264" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="265" fillId="266" borderId="265" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="266" fillId="267" borderId="266" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="267" fillId="268" borderId="267" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="192" borderId="191" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -7985,8 +7980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G56" sqref="G10:G56"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7995,8 +7990,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="267" t="s">
-        <v>57</v>
+      <c r="A1" s="266" t="s">
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -8640,264 +8635,264 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="190" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="191">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="267" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="190">
         <v>1.43</v>
       </c>
-      <c r="C39" s="192">
+      <c r="C39" s="191">
         <v>1.43</v>
       </c>
-      <c r="D39" s="193">
+      <c r="D39" s="192">
         <v>1.52</v>
       </c>
-      <c r="E39" s="194">
+      <c r="E39" s="193">
         <v>1.52</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="195" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="196">
+      <c r="A40" s="194" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="195">
         <v>0.69299999999999995</v>
       </c>
-      <c r="C40" s="197">
+      <c r="C40" s="196">
         <v>0.67200000000000004</v>
       </c>
-      <c r="D40" s="198">
+      <c r="D40" s="197">
         <v>0.69899999999999995</v>
       </c>
-      <c r="E40" s="199">
+      <c r="E40" s="198">
         <v>0.68700000000000006</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="200" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="201">
+      <c r="A41" s="199" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="200">
         <v>0.61699999999999999</v>
       </c>
-      <c r="C41" s="202">
+      <c r="C41" s="201">
         <v>0.59699999999999998</v>
       </c>
-      <c r="D41" s="203">
+      <c r="D41" s="202">
         <v>0.63100000000000001</v>
       </c>
-      <c r="E41" s="204">
+      <c r="E41" s="203">
         <v>0.625</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="205" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="206">
+      <c r="A42" s="204" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="205">
         <v>1</v>
       </c>
-      <c r="C42" s="207">
+      <c r="C42" s="206">
         <v>1</v>
       </c>
-      <c r="D42" s="208">
+      <c r="D42" s="207">
         <v>1</v>
       </c>
-      <c r="E42" s="209">
+      <c r="E42" s="208">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="210" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="211" t="s">
+      <c r="A43" s="209" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="210" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="212" t="s">
+      <c r="C43" s="211" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="213" t="s">
+      <c r="D43" s="212" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="214" t="s">
+      <c r="E43" s="213" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="215" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="216">
+      <c r="A44" s="214" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="215">
         <v>24.7</v>
       </c>
-      <c r="C44" s="217">
+      <c r="C44" s="216">
         <v>27</v>
       </c>
-      <c r="D44" s="218">
+      <c r="D44" s="217">
         <v>25.6</v>
       </c>
-      <c r="E44" s="219">
+      <c r="E44" s="218">
         <v>24.2</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="220" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="221">
+      <c r="A45" s="219" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="220">
         <v>0.58599999999999997</v>
       </c>
-      <c r="C45" s="222">
+      <c r="C45" s="221">
         <v>0.60699999999999998</v>
       </c>
-      <c r="D45" s="223">
+      <c r="D45" s="222">
         <v>0.63800000000000001</v>
       </c>
-      <c r="E45" s="224">
+      <c r="E45" s="223">
         <v>0.65700000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="225" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="226">
+      <c r="A46" s="224" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="225">
         <v>0.443</v>
       </c>
-      <c r="C46" s="227">
+      <c r="C46" s="226">
         <v>0.435</v>
       </c>
-      <c r="D46" s="228">
+      <c r="D46" s="227">
         <v>0.48099999999999998</v>
       </c>
-      <c r="E46" s="229">
+      <c r="E46" s="228">
         <v>0.51100000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="230" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="231">
+      <c r="A47" s="229" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="230">
         <v>0.33</v>
       </c>
-      <c r="C47" s="232">
+      <c r="C47" s="231">
         <v>0.32</v>
       </c>
-      <c r="D47" s="233">
+      <c r="D47" s="232">
         <v>0.36599999999999999</v>
       </c>
-      <c r="E47" s="234">
+      <c r="E47" s="233">
         <v>0.39200000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="235" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="236">
+      <c r="A48" s="234" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="235">
         <v>0.65900000000000003</v>
       </c>
-      <c r="C48" s="237">
+      <c r="C48" s="236">
         <v>0.63600000000000001</v>
       </c>
-      <c r="D48" s="238">
+      <c r="D48" s="237">
         <v>0.63200000000000001</v>
       </c>
-      <c r="E48" s="239">
+      <c r="E48" s="238">
         <v>0.61499999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="240" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="241">
+      <c r="A49" s="239" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="240">
         <v>0.56499999999999995</v>
       </c>
-      <c r="C49" s="242">
+      <c r="C49" s="241">
         <v>0.53500000000000003</v>
       </c>
-      <c r="D49" s="243">
+      <c r="D49" s="242">
         <v>0.57199999999999995</v>
       </c>
-      <c r="E49" s="244">
+      <c r="E49" s="243">
         <v>0.57399999999999995</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="245" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="246">
+      <c r="A50" s="244" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="245">
         <v>0.214</v>
       </c>
-      <c r="C50" s="247">
+      <c r="C50" s="246">
         <v>0.22600000000000001</v>
       </c>
-      <c r="D50" s="248">
+      <c r="D50" s="247">
         <v>0.24199999999999999</v>
       </c>
-      <c r="E50" s="249">
+      <c r="E50" s="248">
         <v>0.248</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="250" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="251">
+      <c r="A51" s="249" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="250">
         <v>12.1</v>
       </c>
-      <c r="C51" s="252">
+      <c r="C51" s="251">
         <v>12.2</v>
       </c>
-      <c r="D51" s="253">
+      <c r="D51" s="252">
         <v>12.8</v>
       </c>
-      <c r="E51" s="254">
+      <c r="E51" s="253">
         <v>12.4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="255" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="256">
+      <c r="A52" s="254" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="255">
         <v>0.81699999999999995</v>
       </c>
-      <c r="C52" s="257">
+      <c r="C52" s="256">
         <v>0.80400000000000005</v>
       </c>
-      <c r="D52" s="258">
+      <c r="D52" s="257">
         <v>0.89900000000000002</v>
       </c>
-      <c r="E52" s="259">
+      <c r="E52" s="258">
         <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="260" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="261">
+      <c r="A53" s="259" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="260">
         <v>27.3</v>
       </c>
-      <c r="C53" s="262">
+      <c r="C53" s="261">
         <v>30.1</v>
       </c>
-      <c r="D53" s="263">
+      <c r="D53" s="262">
         <v>31.1</v>
       </c>
-      <c r="E53" s="264">
+      <c r="E53" s="263">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="265"/>
-      <c r="F55" s="266"/>
+      <c r="A55" s="264"/>
+      <c r="F55" s="265"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>